<commit_message>
- Ajout de l'ombrage et du faciès dans le fichier de description des stations - Ajout du fichier de saisie des données de capteurs
</commit_message>
<xml_diff>
--- a/data/Commentaires/Saisie_commentaires_chroniques.xlsx
+++ b/data/Commentaires/Saisie_commentaires_chroniques.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac27/NAS-JB/Outils/Physico-chimie/Thermie/Fiches_notices/Saisie_commentaires/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Fixe-FD39/Nextcloud_FD/NAS-JB/Outils/Physico-chimie/Thermie/Fiches_notices/Notice/notice-thermie/data/Commentaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB984975-89AB-6245-99A5-068935642ABE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53CD97B-994B-0247-B92A-8E35AD17036C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="5460" windowWidth="28100" windowHeight="17440" xr2:uid="{AB8920CC-5D8D-B14A-9EE7-25D96AE1C5F7}"/>
+    <workbookView xWindow="10740" yWindow="460" windowWidth="18060" windowHeight="16740" xr2:uid="{AB8920CC-5D8D-B14A-9EE7-25D96AE1C5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Àpropos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -471,4 +472,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0C529F-6BAA-C34A-B1D4-4799A906B938}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>20201218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>